<commit_message>
Agregue validaciones en las importaciones de Apoyos
</commit_message>
<xml_diff>
--- a/assets/files/apoyos.xlsx
+++ b/assets/files/apoyos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\INSEZAC\Archivos de proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julieta\Dropbox\INSEZAC Residencias\Archivos de proyecto\Catalogos originales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,11 +531,9 @@
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -563,11 +561,9 @@
         <v>1</v>
       </c>
       <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -595,11 +591,9 @@
         <v>1</v>
       </c>
       <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -627,11 +621,9 @@
         <v>1</v>
       </c>
       <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -659,11 +651,9 @@
         <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -691,11 +681,9 @@
         <v>1</v>
       </c>
       <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -723,11 +711,9 @@
         <v>1</v>
       </c>
       <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -755,11 +741,9 @@
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -787,11 +771,9 @@
         <v>1</v>
       </c>
       <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>